<commit_message>
Updated metadata examples in excel
</commit_message>
<xml_diff>
--- a/examples/excel_template_metadata_example.xlsx
+++ b/examples/excel_template_metadata_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinnorgaard/Documents/GitHub/BIDS-converter/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C061A01-1ADF-524E-860D-662869C152B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C583DDD-FE7F-E141-B6E5-ACD67C9A0BB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16700" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>AttenuationCorrection</t>
+  </si>
+  <si>
+    <t>[137Cs]transmission scan-based</t>
+  </si>
+  <si>
+    <t>13:04:42</t>
   </si>
 </sst>
 </file>
@@ -198,7 +207,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07A739-95C2-BD46-B2B0-50E40D980EB4}">
-  <dimension ref="A1:Z46"/>
+  <dimension ref="A1:AA46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,9 +553,10 @@
     <col min="23" max="23" width="26.33203125" customWidth="1"/>
     <col min="24" max="24" width="27.33203125" customWidth="1"/>
     <col min="25" max="26" width="14.83203125" customWidth="1"/>
+    <col min="27" max="27" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -625,8 +635,11 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -663,8 +676,8 @@
       <c r="L2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="2">
-        <v>0.54493055555555558</v>
+      <c r="M2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -705,8 +718,11 @@
       <c r="Z2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P3">
         <v>10</v>
       </c>
@@ -723,7 +739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P4">
         <v>20</v>
       </c>
@@ -731,7 +747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P5">
         <v>30</v>
       </c>
@@ -739,7 +755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P6">
         <v>40</v>
       </c>
@@ -747,7 +763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P7">
         <v>50</v>
       </c>
@@ -755,7 +771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P8">
         <v>60</v>
       </c>
@@ -763,7 +779,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P9">
         <v>80</v>
       </c>
@@ -771,7 +787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P10">
         <v>100</v>
       </c>
@@ -779,7 +795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P11">
         <v>120</v>
       </c>
@@ -787,7 +803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P12">
         <v>140</v>
       </c>
@@ -795,7 +811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P13">
         <v>160</v>
       </c>
@@ -803,7 +819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P14">
         <v>180</v>
       </c>
@@ -811,7 +827,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P15">
         <v>240</v>
       </c>
@@ -819,7 +835,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="P16">
         <v>300</v>
       </c>

</xml_diff>

<commit_message>
Add metadata examples for conversion
</commit_message>
<xml_diff>
--- a/examples/excel_template_metadata_example.xlsx
+++ b/examples/excel_template_metadata_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinnorgaard/Documents/GitHub/BIDS-converter/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C583DDD-FE7F-E141-B6E5-ACD67C9A0BB0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37D9852-5605-6043-ADAD-E16BE0DDF0E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16700" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
@@ -204,10 +204,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07A739-95C2-BD46-B2B0-50E40D980EB4}">
   <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,7 +636,7 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>